<commit_message>
Added the first ValueSets for HearingObservation profile, wip
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-splasch-HearingObservation.xlsx
+++ b/output/StructureDefinition-splasch-HearingObservation.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-03-24T15:01:17-04:00</t>
+    <t>2022-03-24T23:37:25-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -911,7 +911,7 @@
     <t>valueCodeableConcept</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/pacio-splasch/ValueSet/SPLASCHFrequencyObservationVS</t>
+    <t>http://hl7.org/fhir/us/pacio-splasch/ValueSet/SPLASCHHearingObservationValueVS</t>
   </si>
   <si>
     <t>Observation.dataAbsentReason</t>
@@ -1807,7 +1807,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="60.515625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="73.125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="75.8046875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="23.8515625" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
created valuesets SPLASCHPureToneThresholdAudiometryPanel and SPLASCHDiagnosticAudiologyResultsPanel with additional hearing questions
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-splasch-HearingObservation.xlsx
+++ b/output/StructureDefinition-splasch-HearingObservation.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-05T12:11:10-04:00</t>
+    <t>2022-04-15T08:42:50-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -873,6 +873,10 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
+    <t>CodeableConcept
+integer</t>
+  </si>
+  <si>
     <t>Actual result</t>
   </si>
   <si>
@@ -887,9 +891,6 @@
   <si>
     <t xml:space="preserve">type:$this}
 </t>
-  </si>
-  <si>
-    <t>closed</t>
   </si>
   <si>
     <t xml:space="preserve">obs-7
@@ -4564,19 +4565,19 @@
         <v>92</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>189</v>
+        <v>273</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>81</v>
@@ -4613,14 +4614,14 @@
         <v>81</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AB24" s="2"/>
       <c r="AC24" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>278</v>
+        <v>198</v>
       </c>
       <c r="AE24" t="s" s="2">
         <v>272</v>
@@ -4686,16 +4687,16 @@
         <v>189</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>81</v>
@@ -7626,13 +7627,13 @@
         <v>445</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>446</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>81</v>

</xml_diff>

<commit_message>
built sample data, including new instances for hearing profile.
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-splasch-HearingObservation.xlsx
+++ b/output/StructureDefinition-splasch-HearingObservation.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-15T09:25:37-04:00</t>
+    <t>2022-04-15T12:12:07-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -874,7 +874,7 @@
   </si>
   <si>
     <t>CodeableConcept
-integer</t>
+stringinteger</t>
   </si>
   <si>
     <t>Actual result</t>

</xml_diff>

<commit_message>
add dB unit for hearing observations, where appropriate. Fix dates to be 2020
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-splasch-HearingObservation.xlsx
+++ b/output/StructureDefinition-splasch-HearingObservation.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-04-15T12:12:07-04:00</t>
+    <t>2022-04-18T11:35:28-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -873,8 +873,8 @@
     <t>Observation.value[x]</t>
   </si>
   <si>
-    <t>CodeableConcept
-stringinteger</t>
+    <t>Quantity
+CodeableConceptstring</t>
   </si>
   <si>
     <t>Actual result</t>

</xml_diff>